<commit_message>
chore: added A1-A6 evidences
</commit_message>
<xml_diff>
--- a/0xMemoryGrinder/evidence.xlsx
+++ b/0xMemoryGrinder/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="41">
   <si>
     <t xml:space="preserve">TeamName</t>
   </si>
@@ -100,34 +100,58 @@
     <t xml:space="preserve">ClassID</t>
   </si>
   <si>
-    <t xml:space="preserve">tx hash on irisnet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">class id you issued</t>
+    <t xml:space="preserve">EBA375E8376EC8A7B9F6A2D7764B1B677285A9AAB36B9767951D3491358BD0EE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">memoryGrinderNFT</t>
   </si>
   <si>
     <t xml:space="preserve">NFTID</t>
   </si>
   <si>
-    <t xml:space="preserve">nft id you minted</t>
+    <t xml:space="preserve">839A11B01819AB73C62F92FFAD4F29D8D52E9A0194E54D21E47A88BE10757FD9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">memoryGrinderNFT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C76B3E1B8ED504C11A798C56F8DC509BAB631CDF80DE835ECE279A197F168B29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">memoryGrinderNFT2</t>
   </si>
   <si>
     <t xml:space="preserve">ChainID</t>
   </si>
   <si>
-    <t xml:space="preserve">ibc class on dest chain</t>
+    <t xml:space="preserve">C45BE4A18C3E8292A21ED6EA1FCF70463B4B067E8AE46E59776D6834BA16EFE8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stars1wlrqlre4839ulvuzl59xx0f65dlsgpaftqpk6fffj833aknj8wmqaweqd0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elgafar-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1ED16E7DBC2B2CC22461308B033FE7A1C4B5E3BEF8E0D075C1114B099C24E184</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/4E18EE5C009FF59FB9700D26FC5E63F5C9C3DF2944D9798EB478EC30C6E36A8F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uptick_7000-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1C1FCDFDF9D999EBA289305619E958DBE4A4418322F8A7E813EDE2D45201282E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">98A10C000C7559E67E4E5FF4CE92595EAC32E437452FCA9B4038A24A6CB9C9BE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc class on chain</t>
   </si>
   <si>
     <t xml:space="preserve">nft id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dest chain id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tx hash on dest chain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ibc class on chain</t>
   </si>
   <si>
     <t xml:space="preserve">tx hash on that chain</t>
@@ -152,7 +176,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -181,6 +205,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -252,7 +282,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -274,6 +304,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -356,7 +390,7 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -462,10 +496,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -506,10 +540,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -550,10 +584,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -594,10 +628,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -633,25 +667,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -687,25 +721,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -741,25 +775,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -795,25 +829,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -849,25 +883,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -903,25 +937,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -943,12 +977,12 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.87"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1000,25 +1034,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1054,25 +1088,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1109,12 +1143,12 @@
     </row>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1151,12 +1185,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1193,12 +1227,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1235,12 +1269,12 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1259,15 +1293,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.87"/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.01"/>
   </cols>
   <sheetData>
@@ -1284,13 +1319,24 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1312,12 +1358,13 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.87"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.43"/>
   </cols>
@@ -1333,35 +1380,92 @@
         <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>23</v>
+      <c r="D2" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.43"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1369,12 +1473,13 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.87"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.43"/>
   </cols>
@@ -1390,105 +1495,48 @@
         <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+      <c r="D2" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.43"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.87"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.43"/>
@@ -1505,21 +1553,21 @@
         <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1560,10 +1608,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1604,10 +1652,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>34</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix caps error nd redone transfer + transfer back
</commit_message>
<xml_diff>
--- a/0xMemoryGrinder/evidence.xlsx
+++ b/0xMemoryGrinder/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -115,10 +115,10 @@
     <t xml:space="preserve">memoryGrinderNFT1</t>
   </si>
   <si>
-    <t xml:space="preserve">C76B3E1B8ED504C11A798C56F8DC509BAB631CDF80DE835ECE279A197F168B29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">memoryGrinderNFT2</t>
+    <t xml:space="preserve">172C6D84CB7876C27376ECC7D4D408990EB350FB3F4F6C4ABA745499FAAA5C3A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">memoryGrinderNFT4</t>
   </si>
   <si>
     <t xml:space="preserve">ChainID</t>
@@ -130,22 +130,22 @@
     <t xml:space="preserve">stars1wlrqlre4839ulvuzl59xx0f65dlsgpaftqpk6fffj833aknj8wmqaweqd0</t>
   </si>
   <si>
-    <t xml:space="preserve">Elgafar-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1ED16E7DBC2B2CC22461308B033FE7A1C4B5E3BEF8E0D075C1114B099C24E184</t>
+    <t xml:space="preserve">elgafar-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14835E551EF9A9F551030B20D90EDE4AC29A0E0A7E647147EF7F9A45DEC7E0A2</t>
   </si>
   <si>
     <t xml:space="preserve">ibc/4E18EE5C009FF59FB9700D26FC5E63F5C9C3DF2944D9798EB478EC30C6E36A8F</t>
   </si>
   <si>
-    <t xml:space="preserve">Uptick_7000-2</t>
+    <t xml:space="preserve">uptick_7000-2</t>
   </si>
   <si>
     <t xml:space="preserve">1C1FCDFDF9D999EBA289305619E958DBE4A4418322F8A7E813EDE2D45201282E</t>
   </si>
   <si>
-    <t xml:space="preserve">98A10C000C7559E67E4E5FF4CE92595EAC32E437452FCA9B4038A24A6CB9C9BE</t>
+    <t xml:space="preserve">ED35D60216058469285BF3BA9AE2811CE45737312B00CFC110C6C5AF0D547D50</t>
   </si>
   <si>
     <t xml:space="preserve">ibc class on chain</t>
@@ -1296,7 +1296,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1358,13 +1358,13 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="83.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.43"/>
   </cols>
@@ -1416,13 +1416,14 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.01"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="50.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.43"/>
   </cols>
   <sheetData>
@@ -1472,8 +1473,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1508,7 +1509,7 @@
       <c r="C2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1530,15 +1531,15 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="60.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.43"/>
   </cols>
   <sheetData>
@@ -1560,7 +1561,7 @@
       <c r="A2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C2" s="5" t="s">

</xml_diff>